<commit_message>
updating figures and details needed for README
</commit_message>
<xml_diff>
--- a/data_pipeline_inExcel.xlsx
+++ b/data_pipeline_inExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\Dropbox\GitHub\data_pipeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\GitHub\data_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2960087-000A-4FFA-8B08-DFB7229C524F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28873DFF-0496-4FF2-96EC-7BE78F28C0D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8175" xr2:uid="{601F4121-6B15-4DAB-9F8D-B5E17A764040}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8180" activeTab="1" xr2:uid="{601F4121-6B15-4DAB-9F8D-B5E17A764040}"/>
   </bookViews>
   <sheets>
     <sheet name="mergedSections" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>at sea</t>
   </si>
@@ -43,15 +43,9 @@
     <t>Get R script from github.com/BIOS-SCOPE/data_pipeline/R_code</t>
   </si>
   <si>
-    <t>Join_BATS_All_with_master_v2.R</t>
-  </si>
-  <si>
     <t>Get MATLAB scripts from github.com/BIOS-SCOPE/data_pipeline/MATLAB_code</t>
   </si>
   <si>
-    <t>Create_bioscope_files_2022_2023_Krista.m</t>
-  </si>
-  <si>
     <t>Join_discreteData.R</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     </r>
   </si>
   <si>
-    <t>Join_discreteData_v2.R</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -399,6 +390,12 @@
       </rPr>
       <t xml:space="preserve"> use Join_discreteData_v2.R to pull the variables into the bottle file</t>
     </r>
+  </si>
+  <si>
+    <t>Create_bioscope_files_2024_Krista.m</t>
+  </si>
+  <si>
+    <t>Join_discreteData_v3.R</t>
   </si>
 </sst>
 </file>
@@ -891,31 +888,31 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
     <col min="3" max="3" width="106" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -924,36 +921,36 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="26.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -961,63 +958,63 @@
       <c r="C6" s="4"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="15"/>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="16"/>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="15"/>
       <c r="C11" s="7" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="16"/>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="16"/>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -1025,27 +1022,27 @@
       <c r="C14" s="4"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="15"/>
       <c r="C15" s="7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="17"/>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D17" s="14"/>
     </row>
@@ -1066,30 +1063,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9BB768-0C33-466A-87BD-A91485B7023F}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" customWidth="1"/>
     <col min="3" max="3" width="78" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1097,109 +1094,109 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.35">
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+    <row r="17" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.35">
       <c r="C20" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="C23" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding AE2511 to discrete file
</commit_message>
<xml_diff>
--- a/data_pipeline_inExcel.xlsx
+++ b/data_pipeline_inExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\GitHub\data_pipeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\GitHub_niskin\data_pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28873DFF-0496-4FF2-96EC-7BE78F28C0D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3895792-FD4C-4828-BD9B-AC5050EFAF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="8180" activeTab="1" xr2:uid="{601F4121-6B15-4DAB-9F8D-B5E17A764040}"/>
+    <workbookView xWindow="-27525" yWindow="4155" windowWidth="27495" windowHeight="16290" activeTab="1" xr2:uid="{601F4121-6B15-4DAB-9F8D-B5E17A764040}"/>
   </bookViews>
   <sheets>
     <sheet name="mergedSections" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Get MATLAB scripts from github.com/BIOS-SCOPE/data_pipeline/MATLAB_code</t>
   </si>
   <si>
-    <t>Join_discreteData.R</t>
-  </si>
-  <si>
     <t>Assigned to: Rachel Parsons (or Craig Carlson)</t>
   </si>
   <si>
@@ -396,6 +393,9 @@
   </si>
   <si>
     <t>Join_discreteData_v3.R</t>
+  </si>
+  <si>
+    <t>Create_biosscope_files_2026.m</t>
   </si>
 </sst>
 </file>
@@ -587,9 +587,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -627,7 +627,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -733,7 +733,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -875,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -892,27 +892,27 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="106" customWidth="1"/>
-    <col min="4" max="4" width="46.81640625" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -921,36 +921,36 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="4"/>
       <c r="C5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" ht="26.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="5" t="s">
         <v>4</v>
@@ -958,31 +958,31 @@
       <c r="C6" s="4"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="15"/>
       <c r="C7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="16"/>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -990,31 +990,31 @@
       <c r="C10" s="4"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="15"/>
       <c r="C11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="16"/>
       <c r="C12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="16"/>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="5" t="s">
         <v>4</v>
@@ -1022,27 +1022,27 @@
       <c r="C14" s="4"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="15"/>
       <c r="C15" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="16"/>
       <c r="C16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="17"/>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="14"/>
     </row>
@@ -1064,29 +1064,29 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="78" customWidth="1"/>
-    <col min="4" max="4" width="46.81640625" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1094,109 +1094,109 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C10" s="2" t="s">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C16" s="2" t="s">
+    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C23" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>